<commit_message>
Embibe :: Updated Functional and sanity test scripts
</commit_message>
<xml_diff>
--- a/Embibe/test-data/TestData.xlsx
+++ b/Embibe/test-data/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Unique Value</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>GUJCET</t>
+  </si>
+  <si>
+    <t>Sanity_12</t>
+  </si>
+  <si>
+    <t>Accleration</t>
+  </si>
+  <si>
+    <t>Sanity_13</t>
   </si>
 </sst>
 </file>
@@ -527,10 +536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -579,6 +588,25 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Embibe :: Updated SearchHomePage, SearchResultsPage, W_BasePage, W_SuperBasePage and TestData.xlsx
</commit_message>
<xml_diff>
--- a/Embibe/test-data/TestData.xlsx
+++ b/Embibe/test-data/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Unique Value</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Sanity_13</t>
+  </si>
+  <si>
+    <t>HeadersTest</t>
   </si>
 </sst>
 </file>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,6 +751,20 @@
         <v>27</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -757,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Embibe :: Updated Landing, SearchHomep, SearchResults, Base pages and TestData
</commit_message>
<xml_diff>
--- a/Embibe/test-data/TestData.xlsx
+++ b/Embibe/test-data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Unique Value</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>HeadersTest</t>
+  </si>
+  <si>
+    <t>MeasurabilityFlow3</t>
   </si>
 </sst>
 </file>
@@ -654,10 +657,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -762,6 +765,20 @@
         <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>